<commit_message>
updated templates (removed id column)
</commit_message>
<xml_diff>
--- a/public/Indicators_Template.xlsx
+++ b/public/Indicators_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="460" windowWidth="28800" windowHeight="16140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Level</t>
   </si>
@@ -347,28 +344,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Broken Template" error="Warning! You entered data into a cell that does not comply with this template! Please find the cell and remove the data." promptTitle="WARNING" prompt="You are about to enter data into a cell that does not comply with this template! Please do not enter data into this cell." sqref="D1:BES1048576">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Broken Template" error="Warning! You entered data into a cell that does not comply with this template! Please find the cell and remove the data." promptTitle="WARNING" prompt="You are about to enter data into a cell that does not comply with this template! Please do not enter data into this cell." sqref="C1:BER1048576">
       <formula1>""</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>